<commit_message>
configure A/D individual difference
configure A/D individual difference
</commit_message>
<xml_diff>
--- a/M5_DVM_data/ESP32_ADC_Charactristics.xlsx
+++ b/M5_DVM_data/ESP32_ADC_Charactristics.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\M5_Multimeter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\M5Stack_DVM\M5_DVM_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003D7BCC-2C22-41ED-99BB-8E1351DD5888}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B2C32B-D453-4BCB-B75E-308FF4334786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11445" activeTab="1" xr2:uid="{58BC33EF-26FF-4D97-8AC8-A93305A6D607}"/>
+    <workbookView xWindow="4380" yWindow="750" windowWidth="14580" windowHeight="19215" activeTab="1" xr2:uid="{58BC33EF-26FF-4D97-8AC8-A93305A6D607}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -151,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +169,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,7 +208,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -224,6 +238,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2412,7 +2429,7 @@
   <dimension ref="B2:F63"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="D63" sqref="B2:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2681,7 +2698,7 @@
         <f t="shared" si="2"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="10">
         <v>1084</v>
       </c>
       <c r="D22" s="5">
@@ -2811,7 +2828,7 @@
         <f t="shared" si="2"/>
         <v>2.0000000000000004</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="10">
         <v>2303</v>
       </c>
       <c r="D32" s="5">
@@ -2908,7 +2925,7 @@
         <f t="shared" si="2"/>
         <v>2.7000000000000011</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="10">
         <v>3179</v>
       </c>
       <c r="D39" s="5">
@@ -2947,7 +2964,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000013</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="10">
         <v>3659</v>
       </c>
       <c r="D42" s="5">
@@ -3090,7 +3107,7 @@
         <f t="shared" si="3"/>
         <v>3.1999999999999993</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="10">
         <v>4071</v>
       </c>
       <c r="D53" s="5">

</xml_diff>